<commit_message>
braga + viana + gaia (sem baseline)
braga + viana + gaia (sem baseline)
</commit_message>
<xml_diff>
--- a/data/Braga.xlsx
+++ b/data/Braga.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Dropbox\BIC Beatriz Godinho\Shapefiles cidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED4D5C1-66D0-4E50-997A-07E383FDF140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E11DF-5BC0-4653-A37B-EB19633652C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metrics" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="1180">
   <si>
     <t>Building_Name</t>
   </si>
@@ -25839,7 +25839,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -25894,9 +25896,6 @@
       <c r="H2" t="s">
         <v>1157</v>
       </c>
-      <c r="I2" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -25923,9 +25922,6 @@
       <c r="H3" t="s">
         <v>1157</v>
       </c>
-      <c r="I3" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -25952,9 +25948,6 @@
       <c r="H4" t="s">
         <v>1157</v>
       </c>
-      <c r="I4" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -25981,9 +25974,6 @@
       <c r="H5" t="s">
         <v>1157</v>
       </c>
-      <c r="I5" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -26010,9 +26000,6 @@
       <c r="H6" t="s">
         <v>1157</v>
       </c>
-      <c r="I6" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -26039,9 +26026,6 @@
       <c r="H7" t="s">
         <v>1157</v>
       </c>
-      <c r="I7" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -26068,9 +26052,6 @@
       <c r="H8" t="s">
         <v>1157</v>
       </c>
-      <c r="I8" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -26094,9 +26075,6 @@
       <c r="H9" t="s">
         <v>1158</v>
       </c>
-      <c r="I9" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -26123,9 +26101,6 @@
       <c r="H10" t="s">
         <v>1158</v>
       </c>
-      <c r="I10" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -26152,9 +26127,6 @@
       <c r="H11" t="s">
         <v>1158</v>
       </c>
-      <c r="I11" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -26178,9 +26150,6 @@
       <c r="H12" t="s">
         <v>1159</v>
       </c>
-      <c r="I12" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -26207,9 +26176,6 @@
       <c r="H13" t="s">
         <v>1159</v>
       </c>
-      <c r="I13" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -26236,9 +26202,6 @@
       <c r="H14" t="s">
         <v>1159</v>
       </c>
-      <c r="I14" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -26262,9 +26225,6 @@
       <c r="H15" t="s">
         <v>1160</v>
       </c>
-      <c r="I15" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -26291,11 +26251,8 @@
       <c r="H16" t="s">
         <v>1160</v>
       </c>
-      <c r="I16" t="s">
-        <v>1161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1121</v>
       </c>
@@ -26319,9 +26276,6 @@
       </c>
       <c r="H17" t="s">
         <v>1160</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1161</v>
       </c>
     </row>
   </sheetData>
@@ -26333,7 +26287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
braga + viana + gaia (sem baseline) (#127)
braga + viana + gaia (sem baseline)
</commit_message>
<xml_diff>
--- a/data/Braga.xlsx
+++ b/data/Braga.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Dropbox\BIC Beatriz Godinho\Shapefiles cidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED4D5C1-66D0-4E50-997A-07E383FDF140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E11DF-5BC0-4653-A37B-EB19633652C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metrics" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="1180">
   <si>
     <t>Building_Name</t>
   </si>
@@ -25839,7 +25839,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -25894,9 +25896,6 @@
       <c r="H2" t="s">
         <v>1157</v>
       </c>
-      <c r="I2" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -25923,9 +25922,6 @@
       <c r="H3" t="s">
         <v>1157</v>
       </c>
-      <c r="I3" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -25952,9 +25948,6 @@
       <c r="H4" t="s">
         <v>1157</v>
       </c>
-      <c r="I4" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -25981,9 +25974,6 @@
       <c r="H5" t="s">
         <v>1157</v>
       </c>
-      <c r="I5" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -26010,9 +26000,6 @@
       <c r="H6" t="s">
         <v>1157</v>
       </c>
-      <c r="I6" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -26039,9 +26026,6 @@
       <c r="H7" t="s">
         <v>1157</v>
       </c>
-      <c r="I7" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -26068,9 +26052,6 @@
       <c r="H8" t="s">
         <v>1157</v>
       </c>
-      <c r="I8" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -26094,9 +26075,6 @@
       <c r="H9" t="s">
         <v>1158</v>
       </c>
-      <c r="I9" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -26123,9 +26101,6 @@
       <c r="H10" t="s">
         <v>1158</v>
       </c>
-      <c r="I10" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -26152,9 +26127,6 @@
       <c r="H11" t="s">
         <v>1158</v>
       </c>
-      <c r="I11" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -26178,9 +26150,6 @@
       <c r="H12" t="s">
         <v>1159</v>
       </c>
-      <c r="I12" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -26207,9 +26176,6 @@
       <c r="H13" t="s">
         <v>1159</v>
       </c>
-      <c r="I13" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -26236,9 +26202,6 @@
       <c r="H14" t="s">
         <v>1159</v>
       </c>
-      <c r="I14" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -26262,9 +26225,6 @@
       <c r="H15" t="s">
         <v>1160</v>
       </c>
-      <c r="I15" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -26291,11 +26251,8 @@
       <c r="H16" t="s">
         <v>1160</v>
       </c>
-      <c r="I16" t="s">
-        <v>1161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1121</v>
       </c>
@@ -26319,9 +26276,6 @@
       </c>
       <c r="H17" t="s">
         <v>1160</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1161</v>
       </c>
     </row>
   </sheetData>
@@ -26333,7 +26287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>